<commit_message>
Introduced support for baseline with no norm and social awareness (i.e., no fuzzy inference systems, nor normative reasoning in the bdi). Fixed some bugs here and there. Introduced a state machine that allows to have a response ready for the next user reply. e.g., when asking a question about the news, the robot has the answer to its own question ready.
</commit_message>
<xml_diff>
--- a/data/fuzzy_rules/social_interpretation3/fuzzy_sets_multiple_ref.xlsx
+++ b/data/fuzzy_rules/social_interpretation3/fuzzy_sets_multiple_ref.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ddellanna\surfdrive\PostDoc\Notes\NormsSAR\NormativeBDISAR\data\fuzzy_rules\social_interpretation3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ddellanna\surfdrive\PostDoc\Notes\NormsSAR\NOSAR\data\fuzzy_rules\social_interpretation3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -482,7 +482,7 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1041,10 +1041,10 @@
         <v>0</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F32">
         <v>55</v>

</xml_diff>

<commit_message>
Improved version almost ready for experiimentation with humans. Introduced a minimal baseline, which is going to be used in the experiments and essentially is just a chatbot with no other particular features. Improved the general vocabulary of the robot. Improved the social qualification and the associated rules (now if nao has a subordinate role, this will affect not only suffix and prefix of the sentence but also the way the sentence is said, i.e., faster and with higher voice, based on fuzzy inference). Done some small refactory. Introduced also support to additional animations, and a goodbye social practice where the robot goes to sleep. This commit also contains some changes in the code for the analysis of the results from the simulations about learning.
</commit_message>
<xml_diff>
--- a/data/fuzzy_rules/social_interpretation3/fuzzy_sets_multiple_ref.xlsx
+++ b/data/fuzzy_rules/social_interpretation3/fuzzy_sets_multiple_ref.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="49">
   <si>
     <t>Term</t>
   </si>
@@ -162,6 +162,15 @@
   </si>
   <si>
     <t>ehpc</t>
+  </si>
+  <si>
+    <t>low_speed</t>
+  </si>
+  <si>
+    <t>mid_speed</t>
+  </si>
+  <si>
+    <t>high_speed</t>
   </si>
 </sst>
 </file>
@@ -479,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1041,13 +1050,13 @@
         <v>0</v>
       </c>
       <c r="D32">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="E32">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="F32">
-        <v>55</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1058,16 +1067,16 @@
         <v>22</v>
       </c>
       <c r="C33">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D33">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="E33">
         <v>80</v>
       </c>
       <c r="F33">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1078,7 +1087,7 @@
         <v>22</v>
       </c>
       <c r="C34">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D34">
         <v>100</v>
@@ -1182,6 +1191,66 @@
       </c>
       <c r="E39">
         <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>50</v>
+      </c>
+      <c r="E40">
+        <v>50</v>
+      </c>
+      <c r="F40">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>47</v>
+      </c>
+      <c r="B41" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41">
+        <v>50</v>
+      </c>
+      <c r="D41">
+        <v>100</v>
+      </c>
+      <c r="E41">
+        <v>100</v>
+      </c>
+      <c r="F41">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42" t="s">
+        <v>22</v>
+      </c>
+      <c r="C42">
+        <v>100</v>
+      </c>
+      <c r="D42">
+        <v>150</v>
+      </c>
+      <c r="E42">
+        <v>150</v>
+      </c>
+      <c r="F42">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed some minor bugs. Adjusted the fuzzy rules. Improved vocabulary. This is the version used for the second trial, before starting experimentation.
</commit_message>
<xml_diff>
--- a/data/fuzzy_rules/social_interpretation3/fuzzy_sets_multiple_ref.xlsx
+++ b/data/fuzzy_rules/social_interpretation3/fuzzy_sets_multiple_ref.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="52">
   <si>
     <t>Term</t>
   </si>
@@ -171,6 +171,15 @@
   </si>
   <si>
     <t>high_speed</t>
+  </si>
+  <si>
+    <t>low_tone</t>
+  </si>
+  <si>
+    <t>mid_tone</t>
+  </si>
+  <si>
+    <t>high_tone</t>
   </si>
 </sst>
 </file>
@@ -488,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1244,13 +1253,73 @@
         <v>100</v>
       </c>
       <c r="D42">
+        <v>125</v>
+      </c>
+      <c r="E42">
+        <v>125</v>
+      </c>
+      <c r="F42">
         <v>150</v>
       </c>
-      <c r="E42">
-        <v>150</v>
-      </c>
-      <c r="F42">
-        <v>200</v>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43" t="s">
+        <v>22</v>
+      </c>
+      <c r="C43">
+        <v>70</v>
+      </c>
+      <c r="D43">
+        <v>90</v>
+      </c>
+      <c r="E43">
+        <v>90</v>
+      </c>
+      <c r="F43">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>50</v>
+      </c>
+      <c r="B44" t="s">
+        <v>22</v>
+      </c>
+      <c r="C44">
+        <v>80</v>
+      </c>
+      <c r="D44">
+        <v>100</v>
+      </c>
+      <c r="E44">
+        <v>100</v>
+      </c>
+      <c r="F44">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" t="s">
+        <v>22</v>
+      </c>
+      <c r="C45">
+        <v>100</v>
+      </c>
+      <c r="D45">
+        <v>120</v>
+      </c>
+      <c r="E45">
+        <v>120</v>
+      </c>
+      <c r="F45">
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved several things after trial experiments. Introduced a parrot agent that only repeats what the user says. This will be used to "train" the user (i.e., to let hte user get used to the timming of the robot). Also improved several aspects, in particular related to the timing of different proactive behaviors, and hopefully fixed the issue with the byebye. This version will be quickly tested before starting the first experiment and then will not change (only minor stylish changes will be applied, e.g., commenting the code etc.)
</commit_message>
<xml_diff>
--- a/data/fuzzy_rules/social_interpretation3/fuzzy_sets_multiple_ref.xlsx
+++ b/data/fuzzy_rules/social_interpretation3/fuzzy_sets_multiple_ref.xlsx
@@ -499,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1056,16 +1056,16 @@
         <v>22</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="D32">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="E32">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="F32">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1076,16 +1076,16 @@
         <v>22</v>
       </c>
       <c r="C33">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="D33">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="E33">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="F33">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1096,7 +1096,7 @@
         <v>22</v>
       </c>
       <c r="C34">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D34">
         <v>100</v>
@@ -1230,16 +1230,16 @@
         <v>22</v>
       </c>
       <c r="C41">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="D41">
+        <v>90</v>
+      </c>
+      <c r="E41">
+        <v>90</v>
+      </c>
+      <c r="F41">
         <v>100</v>
-      </c>
-      <c r="E41">
-        <v>100</v>
-      </c>
-      <c r="F41">
-        <v>150</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1250,16 +1250,16 @@
         <v>22</v>
       </c>
       <c r="C42">
+        <v>80</v>
+      </c>
+      <c r="D42">
         <v>100</v>
       </c>
-      <c r="D42">
-        <v>125</v>
-      </c>
       <c r="E42">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="F42">
-        <v>150</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1270,7 +1270,7 @@
         <v>22</v>
       </c>
       <c r="C43">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="D43">
         <v>90</v>

</xml_diff>